<commit_message>
Update status of 2nd,3rd & 4th Nov,20
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vragawade\Documents\D Drive\Qt\Qt Quick\Udemy - Qt Quick and QML For Beginners The Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8841C4F7-7FC9-4F21-BC39-57F56B1D5061}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81CD407-9BC3-4A38-A739-05740E35D816}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>3 videos, 19-21</t>
+  </si>
+  <si>
+    <t>4 videos, 22-25</t>
+  </si>
+  <si>
+    <t>5 videos, 26-30</t>
   </si>
 </sst>
 </file>
@@ -257,9 +266,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -270,25 +276,28 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -574,7 +583,7 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,111 +613,136 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="4">
+      <c r="B3" s="13">
         <v>44135</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>45</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="15">
         <f>SUM(E3:E6)</f>
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>70</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>36</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>28</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>44136</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="8"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="7">
+        <v>44137</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="6">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="8"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="7">
+        <v>44138</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="6">
+        <v>45</v>
+      </c>
+      <c r="F9" s="3">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="8">
-        <v>44137</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="7">
+        <v>44139</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="6">
+        <v>37</v>
+      </c>
+      <c r="F10" s="3">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="8">
-        <v>44138</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F12" s="10">
+      <c r="F12" s="8">
         <f>SUM(F3:F11)</f>
-        <v>179</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -726,7 +760,7 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,35 +772,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="3">
         <v>45</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -775,12 +809,12 @@
       <c r="D4" s="3">
         <v>70</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -789,12 +823,12 @@
       <c r="D5" s="3">
         <v>36</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -803,12 +837,12 @@
       <c r="D6" s="3">
         <v>28</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -817,12 +851,12 @@
       <c r="D7" s="3">
         <v>65</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>43</v>
+      <c r="E7" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -831,12 +865,12 @@
       <c r="D8" s="3">
         <v>37</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>43</v>
+      <c r="E8" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -845,12 +879,12 @@
       <c r="D9" s="3">
         <v>58</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -859,12 +893,12 @@
       <c r="D10" s="3">
         <v>36</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -873,12 +907,12 @@
       <c r="D11" s="3">
         <v>177</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -887,12 +921,12 @@
       <c r="D12" s="3">
         <v>41</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -901,55 +935,55 @@
       <c r="D13" s="3">
         <v>81</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="3">
         <v>97</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="12" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update status of 5th nov
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vragawade\Documents\D Drive\Qt\Qt Quick\Udemy - Qt Quick and QML For Beginners The Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81CD407-9BC3-4A38-A739-05740E35D816}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD90A9C9-4613-4E27-B12E-A0CC95DAB4B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>5 videos, 26-30</t>
+  </si>
+  <si>
+    <t>4 videos, 37-40</t>
+  </si>
+  <si>
+    <t>6 videos, 31-36</t>
   </si>
 </sst>
 </file>
@@ -228,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -251,11 +257,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,6 +323,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,6 +333,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -580,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,7 +654,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="13">
+      <c r="B3" s="14">
         <v>44135</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -625,13 +666,13 @@
       <c r="E3" s="6">
         <v>45</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="16">
         <f>SUM(E3:E6)</f>
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="13"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
@@ -641,10 +682,10 @@
       <c r="E4" s="6">
         <v>70</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="13"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -654,10 +695,10 @@
       <c r="E5" s="6">
         <v>36</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="13"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -667,17 +708,17 @@
       <c r="E6" s="6">
         <v>28</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>44136</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
@@ -734,24 +775,60 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="3"/>
+      <c r="B11" s="14">
+        <v>44140</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="13">
+        <v>58</v>
+      </c>
+      <c r="F11" s="17">
+        <f>SUM(E11:E12)</f>
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F12" s="8">
-        <f>SUM(F3:F11)</f>
-        <v>281</v>
+      <c r="B12" s="14"/>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="13">
+        <v>36</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F14" s="8">
+        <f>SUM(F3:F13)</f>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F3:F6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F11" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -760,7 +837,7 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -879,8 +956,8 @@
       <c r="D9" s="3">
         <v>58</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>43</v>
+      <c r="E9" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
@@ -893,8 +970,8 @@
       <c r="D10" s="3">
         <v>36</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>43</v>
+      <c r="E10" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
@@ -946,7 +1023,9 @@
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3">
+        <v>91</v>
+      </c>
       <c r="E14" s="12" t="s">
         <v>43</v>
       </c>
@@ -958,7 +1037,9 @@
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3">
+        <v>43</v>
+      </c>
       <c r="E15" s="12" t="s">
         <v>43</v>
       </c>
@@ -970,7 +1051,9 @@
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3">
+        <v>55</v>
+      </c>
       <c r="E16" s="12" t="s">
         <v>43</v>
       </c>
@@ -982,7 +1065,9 @@
       <c r="C17" s="3">
         <v>97</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3">
+        <v>6</v>
+      </c>
       <c r="E17" s="12" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
update status for 9 Nov
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vragawade\Documents\D Drive\Qt\Qt Quick\Udemy - Qt Quick and QML For Beginners The Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD90A9C9-4613-4E27-B12E-A0CC95DAB4B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AA18C1-E64F-471C-9FB6-AE800ABEE311}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Activity" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -179,6 +179,18 @@
   </si>
   <si>
     <t>6 videos, 31-36</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>19 videos,41-59</t>
+  </si>
+  <si>
+    <t>5 videos,60-64</t>
+  </si>
+  <si>
+    <t>7 videos,65-71</t>
   </si>
 </sst>
 </file>
@@ -202,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +245,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -283,11 +301,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,6 +400,15 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -339,6 +419,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,7 +753,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="14">
+      <c r="B3" s="17">
         <v>44135</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -666,13 +765,13 @@
       <c r="E3" s="6">
         <v>45</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="19">
         <f>SUM(E3:E6)</f>
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
@@ -682,10 +781,10 @@
       <c r="E4" s="6">
         <v>70</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="14"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -695,10 +794,10 @@
       <c r="E5" s="6">
         <v>36</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="14"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,17 +807,17 @@
       <c r="E6" s="6">
         <v>28</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>44136</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
@@ -775,7 +874,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="14">
+      <c r="B11" s="17">
         <v>44140</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -787,13 +886,13 @@
       <c r="E11" s="13">
         <v>58</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="20">
         <f>SUM(E11:E12)</f>
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
@@ -803,22 +902,123 @@
       <c r="E12" s="13">
         <v>36</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="3"/>
+      <c r="B13" s="14">
+        <v>44141</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="15">
+        <v>130</v>
+      </c>
+      <c r="F13" s="16">
+        <v>130</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F14" s="8">
-        <f>SUM(F3:F13)</f>
-        <v>375</v>
+      <c r="B14" s="14">
+        <v>44142</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="14">
+        <v>44143</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="27">
+        <v>44144</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="6">
+        <v>47</v>
+      </c>
+      <c r="F16" s="20">
+        <f>SUM(E16:E17)</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="28"/>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="6">
+        <v>71</v>
+      </c>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="14">
+        <v>44145</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="14">
+        <v>44146</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="6"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="6"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="8">
+        <f>SUM(F3:F21)</f>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="C14:E15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="F16:F17"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F3:F6"/>
@@ -834,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65387CDF-F08C-461E-9D19-B9994B760312}">
-  <dimension ref="B2:E17"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,7 +1048,7 @@
     <col min="5" max="5" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
@@ -862,7 +1062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -876,7 +1076,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -890,7 +1090,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
@@ -904,7 +1104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
@@ -918,7 +1118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
@@ -932,7 +1132,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
@@ -946,7 +1146,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
@@ -960,7 +1160,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
@@ -974,7 +1174,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
@@ -984,11 +1184,11 @@
       <c r="D11" s="3">
         <v>177</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
@@ -998,11 +1198,11 @@
       <c r="D12" s="3">
         <v>41</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
@@ -1016,7 +1216,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1029,8 +1229,12 @@
       <c r="E14" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <f>SUM(D13:D17)</f>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
@@ -1044,7 +1248,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
status updated for 12 Nov,2020
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vragawade\Documents\D Drive\Qt\Qt Quick\Udemy - Qt Quick and QML For Beginners The Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AA18C1-E64F-471C-9FB6-AE800ABEE311}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D492FE4D-5262-4F67-99CE-32867C55DB47}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -191,13 +191,22 @@
   </si>
   <si>
     <t>7 videos,65-71</t>
+  </si>
+  <si>
+    <t>No Work</t>
+  </si>
+  <si>
+    <t>5 videos,72-76</t>
+  </si>
+  <si>
+    <t>4 videos, 77-80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +218,19 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -358,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,6 +428,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -413,31 +474,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -720,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F22"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -753,7 +789,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="17">
+      <c r="B3" s="32">
         <v>44135</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -765,13 +801,13 @@
       <c r="E3" s="6">
         <v>45</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="34">
         <f>SUM(E3:E6)</f>
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="17"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
@@ -781,10 +817,10 @@
       <c r="E4" s="6">
         <v>70</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="17"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -794,10 +830,10 @@
       <c r="E5" s="6">
         <v>36</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="17"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -807,17 +843,17 @@
       <c r="E6" s="6">
         <v>28</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>44136</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
@@ -874,7 +910,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="17">
+      <c r="B11" s="32">
         <v>44140</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -886,13 +922,13 @@
       <c r="E11" s="13">
         <v>58</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="30">
         <f>SUM(E11:E12)</f>
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="27"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
@@ -902,13 +938,13 @@
       <c r="E12" s="13">
         <v>36</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="14">
         <v>44141</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -925,11 +961,11 @@
       <c r="B14" s="14">
         <v>44142</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="16">
         <v>0</v>
       </c>
@@ -938,18 +974,18 @@
       <c r="B15" s="14">
         <v>44143</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="27">
+      <c r="B16" s="28">
         <v>44144</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -958,13 +994,13 @@
       <c r="E16" s="6">
         <v>47</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="30">
         <f>SUM(E16:E17)</f>
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="28"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
@@ -974,44 +1010,95 @@
       <c r="E17" s="6">
         <v>71</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="31"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="14">
         <v>44145</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="16"/>
+      <c r="C18" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="22">
+        <v>0</v>
+      </c>
+      <c r="F18" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="14">
         <v>44146</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="16"/>
+      <c r="C19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="6">
+        <v>39</v>
+      </c>
+      <c r="F19" s="16">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="6"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="16"/>
+      <c r="B20" s="19">
+        <v>44147</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="6">
+        <v>42</v>
+      </c>
+      <c r="F20" s="18">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="6"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="19">
+        <v>44148</v>
+      </c>
+      <c r="C21" s="17"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F22" s="8">
-        <f>SUM(F3:F21)</f>
-        <v>623</v>
+      <c r="B22" s="19">
+        <v>44149</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="6"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="6"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="8">
+        <f>SUM(F3:F24)</f>
+        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -1025,6 +1112,7 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="F11:F12"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="F11" formulaRange="1"/>
@@ -1037,7 +1125,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,8 +1300,8 @@
       <c r="D13" s="3">
         <v>81</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>43</v>
+      <c r="E13" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update work stauts from 13 Nov to 17 Nov
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vragawade\Documents\D Drive\Qt\Qt Quick\Udemy - Qt Quick and QML For Beginners The Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D492FE4D-5262-4F67-99CE-32867C55DB47}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D08C608-6C7C-4003-95A9-6E4DE51BFA33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Activity" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>4 videos, 77-80</t>
+  </si>
+  <si>
+    <t>4 videos, 93-96</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -376,11 +379,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,6 +457,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -474,6 +494,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -756,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,7 +812,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="32">
+      <c r="B3" s="34">
         <v>44135</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -801,13 +824,13 @@
       <c r="E3" s="6">
         <v>45</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="36">
         <f>SUM(E3:E6)</f>
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="32"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
@@ -817,10 +840,10 @@
       <c r="E4" s="6">
         <v>70</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="32"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -830,10 +853,10 @@
       <c r="E5" s="6">
         <v>36</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="32"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -843,17 +866,17 @@
       <c r="E6" s="6">
         <v>28</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>44136</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
@@ -910,7 +933,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="32">
+      <c r="B11" s="34">
         <v>44140</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -922,13 +945,13 @@
       <c r="E11" s="13">
         <v>58</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="32">
         <f>SUM(E11:E12)</f>
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="28"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
@@ -938,7 +961,7 @@
       <c r="E12" s="13">
         <v>36</v>
       </c>
-      <c r="F12" s="31"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="14">
@@ -961,11 +984,11 @@
       <c r="B14" s="14">
         <v>44142</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="16">
         <v>0</v>
       </c>
@@ -974,15 +997,15 @@
       <c r="B15" s="14">
         <v>44143</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
       <c r="F15" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="28">
+      <c r="B16" s="30">
         <v>44144</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -994,13 +1017,13 @@
       <c r="E16" s="6">
         <v>47</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="32">
         <f>SUM(E16:E17)</f>
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="29"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1010,7 +1033,7 @@
       <c r="E17" s="6">
         <v>71</v>
       </c>
-      <c r="F17" s="31"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="14">
@@ -1067,42 +1090,106 @@
       <c r="B21" s="19">
         <v>44148</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="16"/>
+      <c r="C21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="6">
+        <v>55</v>
+      </c>
+      <c r="F21" s="16">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="19">
         <v>44149</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="18"/>
+      <c r="C22" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="6"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="18"/>
+      <c r="B23" s="25">
+        <v>44150</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="6"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="3"/>
+      <c r="B24" s="25">
+        <v>44151</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F25" s="8">
-        <f>SUM(F3:F24)</f>
-        <v>704</v>
+      <c r="B25" s="25">
+        <v>44152</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="25">
+        <v>44153</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="24"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="6"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="6"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F29" s="8">
+        <f>SUM(F3:F28)</f>
+        <v>759</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="C14:E15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="F16:F17"/>
@@ -1124,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65387CDF-F08C-461E-9D19-B9994B760312}">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1346,8 +1433,8 @@
       <c r="D16" s="3">
         <v>55</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>43</v>
+      <c r="E16" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update status for 21 Nov
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vragawade\Documents\D Drive\Qt\Qt Quick\Udemy - Qt Quick and QML For Beginners The Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D08C608-6C7C-4003-95A9-6E4DE51BFA33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4F3049-1DED-48D1-A738-784CBAF64FE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>4 videos, 93-96</t>
+  </si>
+  <si>
+    <t>3 videos, 90-92</t>
+  </si>
+  <si>
+    <t>create project on Networking demo</t>
+  </si>
+  <si>
+    <t>download ebook &amp; pdf from qmlbook.github.io</t>
   </si>
 </sst>
 </file>
@@ -394,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -463,6 +472,15 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -494,9 +512,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -779,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F29"/>
+  <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -812,7 +827,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="34">
+      <c r="B3" s="37">
         <v>44135</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -824,13 +839,13 @@
       <c r="E3" s="6">
         <v>45</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="39">
         <f>SUM(E3:E6)</f>
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="34"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
@@ -840,10 +855,10 @@
       <c r="E4" s="6">
         <v>70</v>
       </c>
-      <c r="F4" s="36"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="34"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -853,10 +868,10 @@
       <c r="E5" s="6">
         <v>36</v>
       </c>
-      <c r="F5" s="36"/>
+      <c r="F5" s="39"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="34"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -866,17 +881,17 @@
       <c r="E6" s="6">
         <v>28</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="39"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>44136</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
@@ -933,7 +948,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="34">
+      <c r="B11" s="37">
         <v>44140</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -945,13 +960,13 @@
       <c r="E11" s="13">
         <v>58</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="35">
         <f>SUM(E11:E12)</f>
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="30"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
@@ -961,7 +976,7 @@
       <c r="E12" s="13">
         <v>36</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="14">
@@ -984,11 +999,11 @@
       <c r="B14" s="14">
         <v>44142</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="16">
         <v>0</v>
       </c>
@@ -997,15 +1012,15 @@
       <c r="B15" s="14">
         <v>44143</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="30">
+      <c r="B16" s="33">
         <v>44144</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -1017,13 +1032,13 @@
       <c r="E16" s="6">
         <v>47</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="35">
         <f>SUM(E16:E17)</f>
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="31"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1033,7 +1048,7 @@
       <c r="E17" s="6">
         <v>71</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="14">
@@ -1107,11 +1122,11 @@
       <c r="B22" s="19">
         <v>44149</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="18">
         <v>0</v>
       </c>
@@ -1120,11 +1135,11 @@
       <c r="B23" s="25">
         <v>44150</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="24">
         <v>0</v>
       </c>
@@ -1133,11 +1148,11 @@
       <c r="B24" s="25">
         <v>44151</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30"/>
       <c r="F24" s="24">
         <v>0</v>
       </c>
@@ -1146,11 +1161,11 @@
       <c r="B25" s="25">
         <v>44152</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="24">
         <v>0</v>
       </c>
@@ -1159,38 +1174,109 @@
       <c r="B26" s="25">
         <v>44153</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="24"/>
+      <c r="C26" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="22">
+        <v>0</v>
+      </c>
+      <c r="F26" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="6"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="18"/>
+      <c r="B27" s="27">
+        <v>44154</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="22">
+        <v>0</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="6"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="3"/>
+      <c r="B28" s="27">
+        <v>44155</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="6">
+        <v>43</v>
+      </c>
+      <c r="F28" s="18">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F29" s="8">
-        <f>SUM(F3:F28)</f>
-        <v>759</v>
+      <c r="B29" s="33">
+        <v>44156</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="34"/>
+      <c r="C30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0</v>
+      </c>
+      <c r="F30" s="36"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="27">
+        <v>44157</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="26"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="6"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F33" s="8">
+        <f>SUM(F3:F32)</f>
+        <v>802</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C14:E15"/>
+  <mergeCells count="14">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="F29:F30"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="B3:B6"/>
@@ -1198,6 +1284,11 @@
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C14:E15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1212,7 +1303,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1419,8 +1510,8 @@
       <c r="D15" s="3">
         <v>43</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>43</v>
+      <c r="E15" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">

</xml_diff>